<commit_message>
update bom to include motors + gt2 pulley
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B09B7F2XM3/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40mm stepper motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B07SQNYZDY/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;th=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GT2 Timing Belt Pulley 20 tooth, 6mm width, 5mm bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aliexpress.com/item/10000046456013.html?spm=a2g0o.productlist.main.5.59ba2648jXfmXx&amp;algo_pvid=3f3436a0-e6bd-49ab-8fd0-6cb43f8f0c6e&amp;aem_p4p_detail=2023041223572512566913022360240000127032&amp;algo_exp_id=3f3436a0-e6bd-49ab-8fd0-6cb43f8f0c6e-2&amp;pdp_npi=3%40dis%21EUR%212.06%211.44%21%21%21%21%21%402145279016813690456322177d0715%2112000025024121597%21sea%21NL%212329305485&amp;curPageLogUid=09OYRIFzKRYK&amp;ad_pvid=2023041223572512566913022360240000127032_3&amp;ad_pvid=2023041223572512566913022360240000127032_3</t>
   </si>
 </sst>
 </file>
@@ -85,6 +100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,12 +122,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -169,16 +187,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,81 +281,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="116.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="116.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -344,6 +388,8 @@
     <hyperlink ref="C5" r:id="rId4" display="https://www.amazon.nl/-/en/gp/product/B086JYFXPW/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1"/>
     <hyperlink ref="C6" r:id="rId5" display="https://www.amazon.nl/-/en/gp/product/B08M5TSLCN/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1"/>
     <hyperlink ref="C7" r:id="rId6" display="https://www.amazon.nl/-/en/gp/product/B09B7F2XM3/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1"/>
+    <hyperlink ref="C8" r:id="rId7" display="https://www.amazon.nl/-/en/gp/product/B07SQNYZDY/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;th=1"/>
+    <hyperlink ref="C9" r:id="rId8" display="https://www.aliexpress.com/item/10000046456013.html?spm=a2g0o.productlist.main.5.59ba2648jXfmXx&amp;algo_pvid=3f3436a0-e6bd-49ab-8fd0-6cb43f8f0c6e&amp;aem_p4p_detail=2023041223572512566913022360240000127032&amp;algo_exp_id=3f3436a0-e6bd-49ab-8fd0-6cb43f8f0c6e-2&amp;pdp_npi=3%40dis%21EUR%212.06%211.44%21%21%21%21%21%402145279016813690456322177d0715%2112000025024121597%21sea%21NL%212329305485&amp;curPageLogUid=09OYRIFzKRYK&amp;ad_pvid=2023041223572512566913022360240000127032_3&amp;ad_pvid=2023041223572512566913022360240000127032_3"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Ender 3 S1 Corexz v2.1
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">GT2 Belt – 6mm wide</t>
   </si>
   <si>
-    <t xml:space="preserve">5m</t>
+    <t xml:space="preserve">4m</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.nl/gp/product/B07QNWJ1XC/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">F695 2RS Bearing 5*13*4 </t>
   </si>
   <si>
-    <t xml:space="preserve">x20</t>
+    <t xml:space="preserve">x28</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.aliexpress.com/item/33001186278.html?spm=a2g0o.order_list.order_list_main.40.3dee1802y3Ko3C</t>
@@ -55,13 +55,13 @@
     <t xml:space="preserve">https://www.aliexpress.com/item/32917948919.html?spm=a2g0o.order_list.order_list_main.49.3dee1802y3Ko3C</t>
   </si>
   <si>
-    <t xml:space="preserve">20 Series T Nuts M3 M4 M5 T Slot Nuts</t>
+    <t xml:space="preserve">20 Series T Nuts M5 T Slot Nuts</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B086JYFXPW/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
-    <t xml:space="preserve">M4 M5 M6 Hex Socket Bolts / Nuts</t>
+    <t xml:space="preserve">M3 M5 Hex Socket Bolts / Nuts</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B08M5TSLCN/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B09B7F2XM3/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
-    <t xml:space="preserve">40mm stepper motors</t>
+    <t xml:space="preserve">NEMA17 stepper motors</t>
   </si>
   <si>
     <t xml:space="preserve">x2</t>
@@ -284,7 +284,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -330,6 +330,9 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -362,7 +365,7 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -373,7 +376,7 @@
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">

</xml_diff>

<commit_message>
minor update to bom.xlsx
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -52,16 +52,25 @@
     <t xml:space="preserve">Stainless steel Flat Washer 5x10 – 1mm thick</t>
   </si>
   <si>
+    <t xml:space="preserve">x32</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.aliexpress.com/item/32917948919.html?spm=a2g0o.order_list.order_list_main.49.3dee1802y3Ko3C</t>
   </si>
   <si>
     <t xml:space="preserve">20 Series T Nuts M5 T Slot Nuts</t>
   </si>
   <si>
+    <t xml:space="preserve">x8</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B086JYFXPW/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
   </si>
   <si>
-    <t xml:space="preserve">M3 M5 Hex Socket Bolts / Nuts</t>
+    <t xml:space="preserve">M3 M5 Hex Socket Bolts / Nuts (5mm – 30mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x20</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.nl/-/en/gp/product/B08M5TSLCN/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
@@ -284,12 +293,12 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="64.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="116.41"/>
   </cols>
   <sheetData>
@@ -330,57 +339,63 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update number of bearings required
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -43,16 +43,13 @@
     <t xml:space="preserve">F695 2RS Bearing 5*13*4 </t>
   </si>
   <si>
-    <t xml:space="preserve">x28</t>
+    <t xml:space="preserve">x32</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.aliexpress.com/item/33001186278.html?spm=a2g0o.order_list.order_list_main.40.3dee1802y3Ko3C</t>
   </si>
   <si>
     <t xml:space="preserve">Stainless steel Flat Washer 5x10 – 1mm thick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x32</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.aliexpress.com/item/32917948919.html?spm=a2g0o.order_list.order_list_main.49.3dee1802y3Ko3C</t>
@@ -293,7 +290,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -340,62 +337,62 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>